<commit_message>
Updated diary as of 17 March 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="198">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t xml:space="preserve">Deon printed the UML diagram and taped everything together. It’s as messy as we expected. We chose which components to highlight. We wrote up on where the components fit in the UML diagram.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I came in 30 minutes early. Teammates came 40 minutes late. People are busy and traffic is not nice. The difference in time gives a few moments to breathe and observe the lab.</t>
   </si>
   <si>
     <t xml:space="preserve">1910-1945</t>
@@ -612,16 +609,13 @@
     <t xml:space="preserve">More tired than usual. Nutrition and exercise aren’t the issue; something else is wrong. Brain needs rest, and yet I am so used to working actively that I am more comfortable doing something rather than sitting idly.</t>
   </si>
   <si>
-    <t xml:space="preserve">14 Mar 2020 (Tu)</t>
-  </si>
-  <si>
     <t xml:space="preserve">2340-0000</t>
   </si>
   <si>
     <t xml:space="preserve">Feeling better.</t>
   </si>
   <si>
-    <t xml:space="preserve">15 Mar 2020</t>
+    <t xml:space="preserve">15 Mar 2020 (Su)</t>
   </si>
   <si>
     <t xml:space="preserve">0000-1235</t>
@@ -631,6 +625,39 @@
   </si>
   <si>
     <t xml:space="preserve">Most of the test cases in Runelite are surprisingly simple for a large game with a GUI. So it doesn’t seem as scary as I expected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1630-1650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resubmit hw5 and study for possible final exam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resubmitted hw5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Mar 2020 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0100-0210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My mind was deep into Lord of the Rings part 3 when the computer rang;  Thuc and Deon went online and continued working on the project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1615-1850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000-0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Mar 2020 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We did not procrastinate on this homework. There were some problems writing and running test cases, especially since they were for the second pull request.</t>
   </si>
 </sst>
 </file>
@@ -955,8 +982,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E63" activeCellId="0" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1365,25 +1392,23 @@
         <v>77</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="8" t="s">
-        <v>78</v>
-      </c>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
@@ -1393,26 +1418,26 @@
         <v>69</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="E25" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>22</v>
@@ -1427,50 +1452,50 @@
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>21</v>
@@ -1479,43 +1504,43 @@
         <v>22</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="G30" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" s="8" t="str">
         <f aca="false">C30</f>
@@ -1526,17 +1551,17 @@
         <v>Work on fourth lecture’s homework while simutaneously paying attention to the 261 lecture</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>42</v>
@@ -1554,28 +1579,28 @@
     </row>
     <row r="33" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>21</v>
@@ -1584,67 +1609,67 @@
         <v>22</v>
       </c>
       <c r="D34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="G35" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="C36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="F36" s="8" t="str">
         <f aca="false">F35</f>
         <v>I don’t procrastinate out of laziness; the past week or so were full of chaos, both in and out of academia. On the bright side, the lecture recordings help tremendously with the studying.</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>22</v>
@@ -1654,16 +1679,16 @@
         <v>Study for today’s midterm</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>21</v>
@@ -1672,39 +1697,39 @@
         <v>22</v>
       </c>
       <c r="D38" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>129</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D39" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>42</v>
@@ -1714,37 +1739,37 @@
         <v>Supertask by working on latest homework, harassment training, and 264 lab at the same time</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D41" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="G41" s="10" t="s">
         <v>137</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>21</v>
@@ -1753,59 +1778,59 @@
         <v>22</v>
       </c>
       <c r="D42" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>140</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="10"/>
     </row>
     <row r="43" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="C43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" s="8" t="s">
+      <c r="E43" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>144</v>
       </c>
       <c r="G43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>146</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D44" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>148</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>21</v>
@@ -1814,80 +1839,80 @@
         <v>22</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>152</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E46" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="G46" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B47" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B48" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" s="8" t="s">
+      <c r="E48" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>21</v>
@@ -1896,7 +1921,7 @@
         <v>22</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
@@ -1904,31 +1929,31 @@
     </row>
     <row r="50" customFormat="false" ht="264.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>169</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>42</v>
@@ -1943,28 +1968,28 @@
     </row>
     <row r="52" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="8" t="s">
+      <c r="E52" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F52" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>172</v>
       </c>
       <c r="G52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>21</v>
@@ -1973,7 +1998,7 @@
         <v>22</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
@@ -1981,26 +2006,26 @@
     </row>
     <row r="54" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="C54" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>21</v>
@@ -2009,7 +2034,7 @@
         <v>22</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
@@ -2017,29 +2042,29 @@
     </row>
     <row r="56" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>180</v>
-      </c>
       <c r="C56" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>22</v>
@@ -2051,15 +2076,15 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>22</v>
@@ -2069,57 +2094,108 @@
         <v>Work on homework for ninth lecture</v>
       </c>
       <c r="E58" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="C59" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="G58" s="8"/>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
+      <c r="E59" s="8" t="s">
+        <v>189</v>
+      </c>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
+    <row r="60" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>175</v>
+      </c>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
+      <c r="G60" s="8" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
+      <c r="A61" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="8" t="str">
+        <f aca="false">D60</f>
+        <v>Work on homework for ninth lecture</v>
+      </c>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
+      <c r="A62" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="8" t="str">
+        <f aca="false">D61</f>
+        <v>Work on homework for ninth lecture</v>
+      </c>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+    <row r="63" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="8" t="str">
+        <f aca="false">D62</f>
+        <v>Work on homework for ninth lecture</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
+      <c r="G63" s="8" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8"/>

</xml_diff>